<commit_message>
Fixed bug in tax rate extraction
</commit_message>
<xml_diff>
--- a/Analysis/v2 Output Excel/ggppa_progressivity_results_v2.xlsx
+++ b/Analysis/v2 Output Excel/ggppa_progressivity_results_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zctpj17_ucl_ac_uk/Documents/ECON0053 Economics of Tax Policy/Grp Project/Quantitative/GPT PRO/v2 Output Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zctpj17_ucl_ac_uk/Documents/ECON0053 Economics of Tax Policy/Grp Project/Quantitative/Analysis/v2 Output Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{9FEC0CA0-47F8-9C4C-B03C-C23C4292F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E29EDF3B-BAB8-3745-80C4-3FEC88EBE0CE}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{9FEC0CA0-47F8-9C4C-B03C-C23C4292F61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A08B28-0188-344C-871B-BBD80A318264}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="21280" xr2:uid="{220E2251-7415-0C43-A613-EEF453A3BAD9}"/>
   </bookViews>
@@ -1083,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A570435D-4B25-DE4F-A108-299E5B27D444}">
   <dimension ref="A1:AJ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,7 +1166,7 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">

</xml_diff>